<commit_message>
led buzzer .h .cpp ok
</commit_message>
<xml_diff>
--- a/材料表.xlsx
+++ b/材料表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyouchen/Documents/Arduino/uCup_NFC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C565942-5B0F-E249-825E-EA2275C74FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3724433C-1BA0-F042-ABDE-E02AD1EFE5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="1520" windowWidth="28260" windowHeight="17560" xr2:uid="{361DD9CE-442D-8D4B-8DB9-DA2E3DA372F3}"/>
   </bookViews>
@@ -55,22 +55,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>杜邦簧片(母)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>排針(公)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>排針(母)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>38*20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>杜邦塑膠殼(4pin)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -107,18 +95,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>219(運費30)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5*20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>219*20=4380</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>95*20=1900</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -127,38 +107,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2*20=40</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2元/5個</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3元/40個1排</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>40排</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3*40=120</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4元/40個1排</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20排</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4*20=80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>20個</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,7 +135,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(4+7+4+2)*20</t>
+    <t>245(運費0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>245*20=4900</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杜邦簧片(公)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3元/5個</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*20=60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(19+19+4+8+4+2)*20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4*40=160</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杜邦塑膠殼(8pin)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>42個</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8*42=336</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25片</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4335A46E-75B0-B84A-AA52-5CB2C2D7551A}">
-  <dimension ref="D5:K16"/>
+  <dimension ref="D5:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="193" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="193" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -563,25 +563,28 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="4:11">
       <c r="E6" t="s">
         <v>2</v>
       </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
       <c r="H6">
         <v>20</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="4:11">
@@ -612,7 +615,7 @@
         <v>50</v>
       </c>
       <c r="K8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="4:11">
@@ -629,112 +632,111 @@
         <v>95</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="4:11">
       <c r="E10" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11">
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="4:11">
       <c r="E12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="4:11">
       <c r="E13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="K13" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="4:11">
       <c r="E14" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="4:11">
       <c r="D15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="4:11">
       <c r="E16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11">
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17">
+        <v>40</v>
+      </c>
+      <c r="H17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="K6:K7"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>